<commit_message>
Release QRPH.PCC 1.0.0 for TI
</commit_message>
<xml_diff>
--- a/QRPH/CCG/CodeSystem-ccg-card-type-cs.xlsx
+++ b/QRPH/CCG/CodeSystem-ccg-card-type-cs.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>1.0.0-comment</t>
+    <t>1.0.0</t>
   </si>
   <si>
     <t>Name</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-05-20T16:28:52-05:00</t>
+    <t>2025-10-02T10:26:47-05:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>